<commit_message>
clean level and game end mechanic
</commit_message>
<xml_diff>
--- a/data/building_oib_16linie.xlsx
+++ b/data/building_oib_16linie.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F6E657-AC7B-41CC-A95C-B8872F1279B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21496979-E521-42C3-85CF-D64181005DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-3072" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -175,10 +175,10 @@
     <t>€/m²BGF</t>
   </si>
   <si>
-    <t>Außenwand (netto)</t>
-  </si>
-  <si>
     <t>Fenster</t>
+  </si>
+  <si>
+    <t>Aussenwand</t>
   </si>
 </sst>
 </file>
@@ -513,16 +513,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -533,7 +533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -556,7 +556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -567,7 +567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -578,7 +578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -599,16 +599,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,9 +622,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>752.64</v>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -664,9 +664,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>322.56</v>

</xml_diff>